<commit_message>
Test desging for Wallet updated
</commit_message>
<xml_diff>
--- a/TestDesign/CheckList_wallet.xlsx
+++ b/TestDesign/CheckList_wallet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\OneDrive\Escritorio\AQA Bootcamp\Tasks\HTTP-Task\UserService-WalletService_BackendAutoTests\TestDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439583D5-0136-4065-96DB-ABCDDFBBDFD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E2677D-722E-4BD0-A1B1-D16CF4ED2BA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28164" yWindow="960" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WalletServiceTestIdeas" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="82">
   <si>
     <t>N</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Status 500, Body: "Not active user"</t>
   </si>
   <si>
-    <t>Same as 1</t>
-  </si>
-  <si>
     <t>Status 200, Balance is 0.</t>
   </si>
   <si>
@@ -238,6 +235,45 @@
   </si>
   <si>
     <t>Status 200, Balance is 10.0</t>
+  </si>
+  <si>
+    <t>Status 200, balance 0.1</t>
+  </si>
+  <si>
+    <t>Status 200, balance 0.0</t>
+  </si>
+  <si>
+    <t>Status 500</t>
+  </si>
+  <si>
+    <t>status 200, correct balance</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>no transactions, active user</t>
+  </si>
+  <si>
+    <t>new user or not active user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status 200, Balance is </t>
+  </si>
+  <si>
+    <t>Status 200, Balance is 0.01</t>
+  </si>
+  <si>
+    <t>status 200,  balance 0.1.</t>
+  </si>
+  <si>
+    <t>Several transactions, User status set to inactive</t>
+  </si>
+  <si>
+    <t>Status 200, returns correct balance.</t>
+  </si>
+  <si>
+    <t>Status 200, Transaction ID GUID</t>
   </si>
 </sst>
 </file>
@@ -278,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,8 +327,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -315,23 +357,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,22 +726,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -707,7 +763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -718,7 +774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -729,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -740,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -751,7 +807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -762,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -773,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -784,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -795,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -806,7 +862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -817,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -828,7 +884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -839,7 +895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -850,7 +906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -861,7 +917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -872,7 +928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -894,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -905,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -916,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -927,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -938,7 +994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -949,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -960,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -971,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -982,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -993,7 +1049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1004,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1015,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1026,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1037,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1048,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1059,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>33</v>
       </c>
@@ -1081,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>34</v>
       </c>
@@ -1092,7 +1148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>35</v>
       </c>
@@ -1103,7 +1159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>36</v>
       </c>
@@ -1114,7 +1170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>37</v>
       </c>
@@ -1125,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>38</v>
       </c>
@@ -1136,7 +1192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>39</v>
       </c>
@@ -1147,7 +1203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>40</v>
       </c>
@@ -1158,7 +1214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>41</v>
       </c>
@@ -1169,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>42</v>
       </c>
@@ -1180,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>43</v>
       </c>
@@ -1202,7 +1258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>44</v>
       </c>
@@ -1213,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>45</v>
       </c>
@@ -1224,7 +1280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>46</v>
       </c>
@@ -1235,7 +1291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>47</v>
       </c>
@@ -1246,7 +1302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>48</v>
       </c>
@@ -1257,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>49</v>
       </c>
@@ -1268,7 +1324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>50</v>
       </c>
@@ -1279,7 +1335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>51</v>
       </c>
@@ -1290,7 +1346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>52</v>
       </c>
@@ -1301,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>53</v>
       </c>
@@ -1312,7 +1368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>54</v>
       </c>
@@ -1323,7 +1379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>55</v>
       </c>
@@ -1334,7 +1390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>56</v>
       </c>
@@ -1344,6 +1400,9 @@
       <c r="C63">
         <v>3</v>
       </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1354,23 +1413,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>57</v>
       </c>
@@ -1396,438 +1456,490 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="5">
         <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4">
-        <v>3</v>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="4">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="D15" s="4">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="8">
+        <v>2</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="D16" s="4">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="D17" s="4">
-        <v>3</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="B19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="D18" s="4">
-        <v>3</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="B23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="B25" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>